<commit_message>
Way better regex for aircraft Note
</commit_message>
<xml_diff>
--- a/DataEntry.xlsx
+++ b/DataEntry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f31e73b004c6ed25/Work/B737-800MPD/B737-800MPD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_6FE161EF2163080A672D4C7E7DAE25C9787862FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78CCBA8D-0406-43C1-8CA1-10276958F188}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="11_6FE161EF2163080A672D4C7E7DAE25C9787862FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EAD89E1-83AD-4B71-B2BA-38C38CEBAD35}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,9 +59,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Aircraft Type:</t>
+  </si>
+  <si>
+    <t>Winglets</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -453,26 +459,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>800</v>
       </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Winglets" prompt="Are Winglets installed: Yes / No" sqref="B2" xr:uid="{42AE951D-9162-45CD-B8D6-E5E8F72A7BCC}">
+      <formula1>"Yes,No,Don't Know"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>